<commit_message>
Organização e estruturação dos dados.
Ajustes e equalização das planilhas dos exercícios de 2023 e 2024, tanto para softwares adquiridos quanto os desenvolvidos internamente.
</commit_message>
<xml_diff>
--- a/Inventário de Ativos Intangíveis/2024/3. Analise de Dados/3.2. Dados/RLT- Medições Ativos Intangíveis 2023-v1.2.xlsx
+++ b/Inventário de Ativos Intangíveis/2024/3. Analise de Dados/3.2. Dados/RLT- Medições Ativos Intangíveis 2023-v1.2.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathasmarques\Downloads\Dashbord_GestaoProdutos\Dashbord_GestaoProdutos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Seplag\Inventário de Ativos Intangíveis\2024\3. Analise de Dados\3.2. Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEB9AF4-8987-4398-861A-28B47E70EC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21075" windowHeight="8100" tabRatio="190"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mensuração" sheetId="1" r:id="rId1"/>
     <sheet name="Dashbords" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mensuração!$B$6:$N$29</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Mensuração!$A$1:$N$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mensuração!$B$6:$O$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Mensuração!$A$1:$O$36</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="80">
   <si>
     <t>Itens</t>
   </si>
@@ -335,12 +336,6 @@
 RELATÓRIO DE AVALIAÇÃO BENS INTANGÍVEIS DESENVOLVIDOS INTERNAMENTE</t>
   </si>
   <si>
-    <t>Frricante</t>
-  </si>
-  <si>
-    <t>STI/SEPLAG</t>
-  </si>
-  <si>
     <t>SEAP</t>
   </si>
   <si>
@@ -365,19 +360,25 @@
     <t>Tipo SW</t>
   </si>
   <si>
-    <t>SW Desenv STI</t>
-  </si>
-  <si>
-    <t>SW Intra SIT</t>
-  </si>
-  <si>
     <t>SW Legado</t>
+  </si>
+  <si>
+    <t>Exercício</t>
+  </si>
+  <si>
+    <t>Fabricante</t>
+  </si>
+  <si>
+    <t>SITEC/SEPLAG</t>
+  </si>
+  <si>
+    <t>SW Desenv SITEC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
@@ -483,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -537,9 +538,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -574,7 +572,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -689,7 +687,7 @@
           <c:showSerName val="0"/>
           <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
@@ -827,7 +825,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-64D2-469E-9952-1BC4B0C5DF61}"/>
               </c:ext>
@@ -871,7 +869,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-64D2-469E-9952-1BC4B0C5DF61}"/>
               </c:ext>
@@ -955,7 +953,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-64D2-469E-9952-1BC4B0C5DF61}"/>
             </c:ext>
@@ -1048,7 +1046,7 @@
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:extLst>
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
@@ -1540,13 +1538,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>209560</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>24849</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>819598</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>210875</xdr:rowOff>
@@ -1556,7 +1554,7 @@
         <xdr:cNvPr id="2" name="Imagem 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1611,7 +1609,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1633,9 +1631,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jonathas Gomes Marques" refreshedDate="44916.659587731483" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="14">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jonathas Gomes Marques" refreshedDate="44916.659587731483" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="14" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B6:M29" sheet="Mensuração"/>
+    <worksheetSource ref="B6:N29" sheet="Mensuração"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Itens" numFmtId="0">
@@ -1910,7 +1908,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17" rowHeaderCaption="Situação">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Tabela dinâmica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17" rowHeaderCaption="Situação">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -2289,1285 +2287,1367 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:P37"/>
+  <dimension ref="B1:Q37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="10" topLeftCell="I17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="10" topLeftCell="M17" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
-      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="3" width="6.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" customWidth="1"/>
+    <col min="15" max="15" width="25.33203125" customWidth="1"/>
+    <col min="16" max="16" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="27" t="s">
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="2:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-    </row>
-    <row r="3" spans="2:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-    </row>
-    <row r="4" spans="2:16" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+    </row>
+    <row r="3" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+    </row>
+    <row r="4" spans="2:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="2:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="2:17" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="N6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="11" t="s">
-        <v>67</v>
-      </c>
       <c r="P6" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>45271</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>181.7</v>
       </c>
-      <c r="J7" s="8">
+      <c r="K7" s="8">
         <v>705.6</v>
       </c>
-      <c r="K7" s="9">
-        <f>I7*J7</f>
+      <c r="L7" s="9">
+        <f>J7*K7</f>
         <v>128207.51999999999</v>
       </c>
-      <c r="L7" s="14">
+      <c r="M7" s="14">
         <v>0.5</v>
       </c>
-      <c r="M7" s="9">
-        <f>K7+(K7*L7)</f>
+      <c r="N7" s="9">
+        <f>L7+(L7*M7)</f>
         <v>192311.27999999997</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="18"/>
+      <c r="P7" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="6">
         <v>45271</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>665</v>
       </c>
-      <c r="J8" s="8">
+      <c r="K8" s="8">
         <v>705.6</v>
       </c>
-      <c r="K8" s="9">
-        <f>I8*J8</f>
+      <c r="L8" s="9">
+        <f>J8*K8</f>
         <v>469224</v>
       </c>
-      <c r="L8" s="14">
+      <c r="M8" s="14">
         <v>0.5</v>
       </c>
-      <c r="M8" s="9">
-        <f t="shared" ref="M8:M30" si="0">K8+(K8*L8)</f>
+      <c r="N8" s="9">
+        <f t="shared" ref="N8:N30" si="0">L8+(L8*M8)</f>
         <v>703836</v>
       </c>
-      <c r="N8" s="18"/>
-      <c r="O8" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O8" s="18"/>
+      <c r="P8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="6">
         <v>45271</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <v>485.4</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>705.6</v>
       </c>
-      <c r="K9" s="9">
-        <f>I9*J9</f>
+      <c r="L9" s="9">
+        <f>J9*K9</f>
         <v>342498.24</v>
       </c>
-      <c r="L9" s="14">
+      <c r="M9" s="14">
         <v>0.75</v>
       </c>
-      <c r="M9" s="9">
+      <c r="N9" s="9">
         <f t="shared" si="0"/>
         <v>599371.91999999993</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P9" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="105" x14ac:dyDescent="0.25">
+      <c r="O9" s="18"/>
+      <c r="P9" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <v>45148</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
         <v>1850</v>
       </c>
-      <c r="J10" s="8">
+      <c r="K10" s="8">
         <v>705.6</v>
       </c>
-      <c r="K10" s="9">
-        <f t="shared" ref="K10:K30" si="1">I10*J10</f>
+      <c r="L10" s="9">
+        <f t="shared" ref="L10:L30" si="1">J10*K10</f>
         <v>1305360</v>
       </c>
-      <c r="L10" s="14">
+      <c r="M10" s="14">
         <v>0.25</v>
       </c>
-      <c r="M10" s="9">
+      <c r="N10" s="9">
         <f t="shared" si="0"/>
         <v>1631700</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="O10" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="O10" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P10" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>45272</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>255.6</v>
       </c>
-      <c r="J11" s="8">
+      <c r="K11" s="8">
         <v>705.6</v>
       </c>
-      <c r="K11" s="9">
+      <c r="L11" s="9">
         <f t="shared" si="1"/>
         <v>180351.36000000002</v>
       </c>
-      <c r="L11" s="14">
+      <c r="M11" s="14">
         <v>0.25</v>
       </c>
-      <c r="M11" s="9">
+      <c r="N11" s="9">
         <f t="shared" si="0"/>
         <v>225439.2</v>
       </c>
-      <c r="N11" s="18"/>
-      <c r="O11" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P11" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O11" s="18"/>
+      <c r="P11" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="6">
+      <c r="I12" s="6">
         <v>45272</v>
       </c>
-      <c r="I12" s="7">
+      <c r="J12" s="7">
         <v>875</v>
       </c>
-      <c r="J12" s="8">
+      <c r="K12" s="8">
         <v>705.6</v>
       </c>
-      <c r="K12" s="9">
+      <c r="L12" s="9">
         <f t="shared" si="1"/>
         <v>617400</v>
       </c>
-      <c r="L12" s="14">
+      <c r="M12" s="14">
         <v>0.75</v>
       </c>
-      <c r="M12" s="9">
+      <c r="N12" s="9">
         <f t="shared" si="0"/>
         <v>1080450</v>
       </c>
-      <c r="N12" s="18"/>
-      <c r="O12" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O12" s="18"/>
+      <c r="P12" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>7</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I13" s="6">
         <v>45272</v>
       </c>
-      <c r="I13" s="7">
+      <c r="J13" s="7">
         <v>456</v>
       </c>
-      <c r="J13" s="8">
+      <c r="K13" s="8">
         <v>705.6</v>
       </c>
-      <c r="K13" s="9">
+      <c r="L13" s="9">
         <f t="shared" si="1"/>
         <v>321753.60000000003</v>
       </c>
-      <c r="L13" s="14">
+      <c r="M13" s="14">
         <v>0.25</v>
       </c>
-      <c r="M13" s="9">
+      <c r="N13" s="9">
         <f t="shared" si="0"/>
         <v>402192.00000000006</v>
       </c>
-      <c r="N13" s="18"/>
-      <c r="O13" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P13" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O13" s="18"/>
+      <c r="P13" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>8</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>45273</v>
       </c>
-      <c r="I14" s="7">
+      <c r="J14" s="7">
         <v>670</v>
       </c>
-      <c r="J14" s="8">
+      <c r="K14" s="8">
         <v>705.6</v>
       </c>
-      <c r="K14" s="9">
+      <c r="L14" s="9">
         <f t="shared" si="1"/>
         <v>472752</v>
       </c>
-      <c r="L14" s="14">
+      <c r="M14" s="14">
         <v>0.75</v>
       </c>
-      <c r="M14" s="9">
+      <c r="N14" s="9">
         <f t="shared" si="0"/>
         <v>827316</v>
       </c>
-      <c r="N14" s="18"/>
-      <c r="O14" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P14" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O14" s="18"/>
+      <c r="P14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>9</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="6">
+      <c r="I15" s="6">
         <v>45272</v>
       </c>
-      <c r="I15" s="7">
+      <c r="J15" s="7">
         <v>749</v>
       </c>
-      <c r="J15" s="8">
+      <c r="K15" s="8">
         <v>705.6</v>
       </c>
-      <c r="K15" s="9">
+      <c r="L15" s="9">
         <f t="shared" si="1"/>
         <v>528494.4</v>
       </c>
-      <c r="L15" s="14">
+      <c r="M15" s="14">
         <v>1</v>
       </c>
-      <c r="M15" s="9">
+      <c r="N15" s="9">
         <f t="shared" si="0"/>
         <v>1056988.8</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P15" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O15" s="18"/>
+      <c r="P15" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="6">
+      <c r="I16" s="6">
         <v>45271</v>
       </c>
-      <c r="I16" s="7">
+      <c r="J16" s="7">
         <v>367</v>
       </c>
-      <c r="J16" s="8">
+      <c r="K16" s="8">
         <v>705.6</v>
       </c>
-      <c r="K16" s="9">
+      <c r="L16" s="9">
         <f t="shared" si="1"/>
         <v>258955.2</v>
       </c>
-      <c r="L16" s="14">
+      <c r="M16" s="14">
         <v>1</v>
       </c>
-      <c r="M16" s="9">
+      <c r="N16" s="9">
         <f t="shared" si="0"/>
         <v>517910.4</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P16" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O16" s="18"/>
+      <c r="P16" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="6">
+      <c r="I17" s="6">
         <v>45271</v>
       </c>
-      <c r="I17" s="7">
+      <c r="J17" s="7">
         <v>80</v>
       </c>
-      <c r="J17" s="8">
+      <c r="K17" s="8">
         <v>705.6</v>
       </c>
-      <c r="K17" s="9">
+      <c r="L17" s="9">
         <f t="shared" si="1"/>
         <v>56448</v>
       </c>
-      <c r="L17" s="14">
+      <c r="M17" s="14">
         <v>1</v>
       </c>
-      <c r="M17" s="9">
+      <c r="N17" s="9">
         <f t="shared" si="0"/>
         <v>112896</v>
       </c>
-      <c r="N17" s="18"/>
-      <c r="O17" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P17" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O17" s="18"/>
+      <c r="P17" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>12</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="6">
+      <c r="I18" s="6">
         <v>45133</v>
       </c>
-      <c r="I18" s="7">
+      <c r="J18" s="7">
         <v>2015</v>
       </c>
-      <c r="J18" s="8">
+      <c r="K18" s="8">
         <v>705.6</v>
       </c>
-      <c r="K18" s="9">
+      <c r="L18" s="9">
         <f t="shared" si="1"/>
         <v>1421784</v>
       </c>
-      <c r="L18" s="14">
+      <c r="M18" s="14">
         <v>0.75</v>
       </c>
-      <c r="M18" s="9">
+      <c r="N18" s="9">
         <f t="shared" si="0"/>
         <v>2488122</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P18" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O18" s="18"/>
+      <c r="P18" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q18" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>13</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="6">
+      <c r="I19" s="6">
         <v>45072</v>
       </c>
-      <c r="I19" s="7">
+      <c r="J19" s="7">
         <v>724</v>
       </c>
-      <c r="J19" s="8">
+      <c r="K19" s="8">
         <v>705.6</v>
       </c>
-      <c r="K19" s="9">
+      <c r="L19" s="9">
         <f t="shared" si="1"/>
         <v>510854.40000000002</v>
       </c>
-      <c r="L19" s="14">
+      <c r="M19" s="14">
         <v>0.25</v>
       </c>
-      <c r="M19" s="9">
+      <c r="N19" s="9">
         <f t="shared" si="0"/>
         <v>638568</v>
       </c>
-      <c r="N19" s="18"/>
-      <c r="O19" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P19" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O19" s="18"/>
+      <c r="P19" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q19" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <v>14</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="6">
+      <c r="I20" s="6">
         <v>45149</v>
       </c>
-      <c r="I20" s="7">
+      <c r="J20" s="7">
         <v>542</v>
       </c>
-      <c r="J20" s="8">
+      <c r="K20" s="8">
         <v>705.6</v>
       </c>
-      <c r="K20" s="9">
+      <c r="L20" s="9">
         <f t="shared" si="1"/>
         <v>382435.2</v>
       </c>
-      <c r="L20" s="14">
+      <c r="M20" s="14">
         <v>0.25</v>
       </c>
-      <c r="M20" s="9">
+      <c r="N20" s="9">
         <f t="shared" si="0"/>
         <v>478044</v>
       </c>
-      <c r="N20" s="18"/>
-      <c r="O20" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P20" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O20" s="18"/>
+      <c r="P20" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>15</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="6">
+      <c r="I21" s="6">
         <v>45202</v>
       </c>
-      <c r="I21" s="7">
+      <c r="J21" s="7">
         <v>277.8</v>
       </c>
-      <c r="J21" s="8">
+      <c r="K21" s="8">
         <v>705.6</v>
       </c>
-      <c r="K21" s="9">
-        <f t="shared" ref="K21:K22" si="2">I21*J21</f>
+      <c r="L21" s="9">
+        <f t="shared" ref="L21:L22" si="2">J21*K21</f>
         <v>196015.68000000002</v>
       </c>
-      <c r="L21" s="14">
+      <c r="M21" s="14">
         <v>0.75</v>
       </c>
-      <c r="M21" s="9">
-        <f t="shared" ref="M21:M22" si="3">K21+(K21*L21)</f>
+      <c r="N21" s="9">
+        <f t="shared" ref="N21:N22" si="3">L21+(L21*M21)</f>
         <v>343027.44000000006</v>
       </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P21" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O21" s="18"/>
+      <c r="P21" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q21" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>16</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="6">
+      <c r="I22" s="6">
         <v>45265</v>
       </c>
-      <c r="I22" s="7">
+      <c r="J22" s="7">
         <v>688.4</v>
       </c>
-      <c r="J22" s="8">
+      <c r="K22" s="8">
         <v>705.6</v>
       </c>
-      <c r="K22" s="9">
+      <c r="L22" s="9">
         <f t="shared" si="2"/>
         <v>485735.04</v>
       </c>
-      <c r="L22" s="14">
+      <c r="M22" s="14">
         <v>0.75</v>
       </c>
-      <c r="M22" s="9">
+      <c r="N22" s="9">
         <f t="shared" si="3"/>
         <v>850036.32</v>
       </c>
-      <c r="N22" s="18"/>
-      <c r="O22" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P22" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O22" s="18"/>
+      <c r="P22" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q22" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <v>17</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="6">
+      <c r="I23" s="6">
         <v>45267</v>
       </c>
-      <c r="I23" s="7">
+      <c r="J23" s="7">
         <v>710.2</v>
       </c>
-      <c r="J23" s="8">
+      <c r="K23" s="8">
         <v>705.6</v>
       </c>
-      <c r="K23" s="9">
-        <f t="shared" ref="K23:K24" si="4">I23*J23</f>
+      <c r="L23" s="9">
+        <f t="shared" ref="L23:L24" si="4">J23*K23</f>
         <v>501117.12000000005</v>
       </c>
-      <c r="L23" s="14">
+      <c r="M23" s="14">
         <v>0.25</v>
       </c>
-      <c r="M23" s="9">
-        <f t="shared" ref="M23:M24" si="5">K23+(K23*L23)</f>
+      <c r="N23" s="9">
+        <f t="shared" ref="N23:N24" si="5">L23+(L23*M23)</f>
         <v>626396.4</v>
       </c>
-      <c r="N23" s="18"/>
-      <c r="O23" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P23" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O23" s="18"/>
+      <c r="P23" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q23" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <v>18</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="6">
+      <c r="I24" s="6">
         <v>45267</v>
       </c>
-      <c r="I24" s="7">
+      <c r="J24" s="7">
         <v>110</v>
       </c>
-      <c r="J24" s="8">
+      <c r="K24" s="8">
         <v>705.6</v>
       </c>
-      <c r="K24" s="9">
+      <c r="L24" s="9">
         <f t="shared" si="4"/>
         <v>77616</v>
       </c>
-      <c r="L24" s="14">
+      <c r="M24" s="14">
         <v>0.25</v>
       </c>
-      <c r="M24" s="9">
+      <c r="N24" s="9">
         <f t="shared" si="5"/>
         <v>97020</v>
       </c>
-      <c r="N24" s="18"/>
-      <c r="O24" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P24" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="18"/>
+      <c r="P24" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q24" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <v>19</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="6">
+      <c r="I25" s="6">
         <v>45272</v>
       </c>
-      <c r="I25" s="7">
+      <c r="J25" s="7">
         <v>335</v>
       </c>
-      <c r="J25" s="8">
+      <c r="K25" s="8">
         <v>705.6</v>
       </c>
-      <c r="K25" s="9">
+      <c r="L25" s="9">
         <f t="shared" si="1"/>
         <v>236376</v>
       </c>
-      <c r="L25" s="14">
+      <c r="M25" s="14">
         <v>1</v>
       </c>
-      <c r="M25" s="9">
+      <c r="N25" s="9">
         <f t="shared" si="0"/>
         <v>472752</v>
       </c>
-      <c r="N25" s="18"/>
-      <c r="O25" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P25" s="22" t="s">
+      <c r="O25" s="18"/>
+      <c r="P25" s="21" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <v>20</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="6">
+      <c r="I26" s="6">
         <v>45272</v>
       </c>
-      <c r="I26" s="7">
+      <c r="J26" s="7">
         <v>46</v>
       </c>
-      <c r="J26" s="8">
+      <c r="K26" s="8">
         <v>705.6</v>
       </c>
-      <c r="K26" s="9">
-        <f t="shared" ref="K26" si="6">I26*J26</f>
+      <c r="L26" s="9">
+        <f t="shared" ref="L26" si="6">J26*K26</f>
         <v>32457.600000000002</v>
       </c>
-      <c r="L26" s="14">
+      <c r="M26" s="14">
         <v>0.25</v>
       </c>
-      <c r="M26" s="9">
-        <f t="shared" ref="M26" si="7">K26+(K26*L26)</f>
+      <c r="N26" s="9">
+        <f t="shared" ref="N26" si="7">L26+(L26*M26)</f>
         <v>40572</v>
       </c>
-      <c r="N26" s="18"/>
-      <c r="O26" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P26" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O26" s="18"/>
+      <c r="P26" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q26" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <v>21</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="6">
+      <c r="I27" s="6">
         <v>45272</v>
       </c>
-      <c r="I27" s="7">
+      <c r="J27" s="7">
         <v>240</v>
       </c>
-      <c r="J27" s="8">
+      <c r="K27" s="8">
         <v>705.6</v>
       </c>
-      <c r="K27" s="9">
+      <c r="L27" s="9">
         <f t="shared" si="1"/>
         <v>169344</v>
       </c>
-      <c r="L27" s="14">
+      <c r="M27" s="14">
         <v>0.25</v>
       </c>
-      <c r="M27" s="9">
+      <c r="N27" s="9">
         <f t="shared" si="0"/>
         <v>211680</v>
       </c>
-      <c r="N27" s="18"/>
-      <c r="O27" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P27" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O27" s="18"/>
+      <c r="P27" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q27" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <v>22</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="6">
+      <c r="I28" s="6">
         <v>45272</v>
       </c>
-      <c r="I28" s="7">
+      <c r="J28" s="7">
         <v>52</v>
       </c>
-      <c r="J28" s="8">
+      <c r="K28" s="8">
         <v>705.6</v>
       </c>
-      <c r="K28" s="9">
+      <c r="L28" s="9">
         <f t="shared" si="1"/>
         <v>36691.200000000004</v>
       </c>
-      <c r="L28" s="14">
+      <c r="M28" s="14">
         <v>0.25</v>
       </c>
-      <c r="M28" s="9">
+      <c r="N28" s="9">
         <f t="shared" si="0"/>
         <v>45864.000000000007</v>
       </c>
-      <c r="N28" s="18"/>
-      <c r="O28" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="P28" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="18"/>
+      <c r="P28" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q28" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="20">
         <v>23</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="6">
+      <c r="I29" s="6">
         <v>45271</v>
       </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="13">
+      <c r="J29" s="12"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="13">
         <v>96833.33</v>
       </c>
-      <c r="N29" s="18"/>
-      <c r="O29" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="P29" s="22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O29" s="18"/>
+      <c r="P29" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q29" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="20">
         <v>24</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>73</v>
+      <c r="C30" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="6">
+      <c r="H30" s="3"/>
+      <c r="I30" s="6">
         <v>45154</v>
       </c>
-      <c r="I30" s="7">
+      <c r="J30" s="7">
         <v>4095</v>
       </c>
-      <c r="J30" s="8">
+      <c r="K30" s="8">
         <v>705.6</v>
       </c>
-      <c r="K30" s="9">
+      <c r="L30" s="9">
         <f t="shared" si="1"/>
         <v>2889432</v>
       </c>
-      <c r="L30" s="14">
+      <c r="M30" s="14">
         <v>1</v>
       </c>
-      <c r="M30" s="9">
+      <c r="N30" s="9">
         <f t="shared" si="0"/>
         <v>5778864</v>
       </c>
-      <c r="N30" s="18"/>
-      <c r="O30" s="22" t="s">
+      <c r="O30" s="18"/>
+      <c r="P30" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q30" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="P30" s="22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="B6:N29"/>
+  <autoFilter ref="B6:O29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="8">
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="D2:N3"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="E2:O3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>
@@ -3576,20 +3656,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
@@ -3597,7 +3677,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
@@ -3605,7 +3685,7 @@
         <v>1856276.875</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -3613,7 +3693,7 @@
         <v>3116534.35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>38</v>
       </c>

</xml_diff>